<commit_message>
Rearranged GASEQ structure and started writing report, almost finished Q1
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/al3615_ic_ac_uk/Documents/ME3/THD/ME3_THD_ThermoCoursework/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="B9D9AC634968205571773F7528B7BC4C4E7EC6E2" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{1B390A6F-41B4-42EC-B6C7-A53368C882EA}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="B9D9AC634968205571773F7528B7BC4C4E7EC6E2" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{14CC9032-5E72-4E13-8E0B-7F90CD3735D8}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="8100" xr2:uid="{8DEAE40B-F84D-48E3-B9B8-1F537C5AE921}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>Temp (K)</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>Position</t>
+  </si>
+  <si>
+    <t>Mass (kg/s)</t>
   </si>
 </sst>
 </file>
@@ -385,15 +388,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC1F890-E0FE-4FD7-B24D-E811BEA20642}">
-  <dimension ref="A2:C27"/>
+  <dimension ref="A2:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -403,8 +410,23 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -414,8 +436,23 @@
       <c r="C3">
         <v>1.0129999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>288.14999999999998</v>
+      </c>
+      <c r="G3">
+        <v>1.0129999999999999</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>23.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -425,8 +462,23 @@
       <c r="C4">
         <v>1.0129999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>288.14999999999998</v>
+      </c>
+      <c r="G4">
+        <v>1.0129999999999999</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>598.70000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -436,8 +488,23 @@
       <c r="C5">
         <v>23.298999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>15</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1.0393380000000001</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <v>17.899999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -447,8 +514,23 @@
       <c r="C6">
         <v>23.298999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>16</v>
+      </c>
+      <c r="F6">
+        <v>428.15</v>
+      </c>
+      <c r="G6">
+        <v>1.0231300000000001</v>
+      </c>
+      <c r="I6">
+        <v>13</v>
+      </c>
+      <c r="J6">
+        <v>254.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -458,8 +540,17 @@
       <c r="C7">
         <v>23.298999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>17</v>
+      </c>
+      <c r="F7">
+        <v>838.65</v>
+      </c>
+      <c r="G7">
+        <v>123.586</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -469,8 +560,17 @@
       <c r="C8">
         <v>23.88654</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>18</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>23.88654</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -480,8 +580,17 @@
       <c r="C9">
         <v>23.298999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>19</v>
+      </c>
+      <c r="F9">
+        <v>838.65</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -491,8 +600,17 @@
       <c r="C10">
         <v>23.298999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>21</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>2.36029</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -502,8 +620,17 @@
       <c r="C11">
         <v>23.298999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>22</v>
+      </c>
+      <c r="F11">
+        <v>292.14999999999998</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -513,8 +640,17 @@
       <c r="C12">
         <v>23.298999999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>23</v>
+      </c>
+      <c r="F12">
+        <v>283.14999999999998</v>
+      </c>
+      <c r="G12">
+        <v>1.0129999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -524,8 +660,17 @@
       <c r="C13">
         <v>23.298999999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>24</v>
+      </c>
+      <c r="F13">
+        <v>321.14999999999998</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -536,7 +681,7 @@
         <v>23.298999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -547,7 +692,7 @@
         <v>23.298999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Finished the muthatruckin work
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/al3615_ic_ac_uk/Documents/ME3/THD/ME3_THD_ThermoCoursework/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\OneDrive - Imperial College London\ME3\THD\ME3_THD_ThermoCoursework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="B9D9AC634968205571773F7528B7BC4C4E7EC6E2" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{14CC9032-5E72-4E13-8E0B-7F90CD3735D8}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="B9D9AC634968205571773F7528B7BC4C4E7EC6E2" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{555FA935-1E28-4856-AF20-B7935FF8CF1C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="8100" xr2:uid="{8DEAE40B-F84D-48E3-B9B8-1F537C5AE921}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="8100" activeTab="1" xr2:uid="{8DEAE40B-F84D-48E3-B9B8-1F537C5AE921}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="14">
   <si>
     <t>Temp (K)</t>
   </si>
@@ -37,6 +38,36 @@
   </si>
   <si>
     <t>Mass (kg/s)</t>
+  </si>
+  <si>
+    <t>Composition</t>
+  </si>
+  <si>
+    <t>91.3% Methane, 5.36% Ethane, 2.83% Nitrogen, 0.5% CO2  and 0.01% O2</t>
+  </si>
+  <si>
+    <t>78.08% N2, 20.95% O2  and 0.93% Ar</t>
+  </si>
+  <si>
+    <t>100% H2O(g)</t>
+  </si>
+  <si>
+    <t>100% H2O(l)</t>
+  </si>
+  <si>
+    <t>51% N2, 28% H2O(g), 7% O2, 5% H2, 3% CO, 3% CO2, 2% CH4, Neg. NOx</t>
+  </si>
+  <si>
+    <t>45% H2, 36% H2O(g), 7% CO, 6% CO2, 5% CH4, 0.5% N2, Neg. NOx</t>
+  </si>
+  <si>
+    <t>61% N2, 29% H2O(g), 7% CO2, 3% O2 , 0.2% NO, Neg. other NOx</t>
+  </si>
+  <si>
+    <t>61% N2, 29% H2O(g), 7% CO2, 3% O2 , 0.002% NO, Neg. other NOx</t>
+  </si>
+  <si>
+    <t>61% N2, 29% H2O(g), 7% CO2, 3% O2 , Neg. NOx</t>
   </si>
 </sst>
 </file>
@@ -52,12 +83,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -72,8 +109,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,19 +426,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC1F890-E0FE-4FD7-B24D-E811BEA20642}">
-  <dimension ref="A2:J27"/>
+  <dimension ref="A2:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" customWidth="1"/>
+    <col min="16" max="16" width="65.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -425,8 +465,11 @@
       <c r="J2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -451,8 +494,18 @@
       <c r="J3">
         <v>23.9</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1"/>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>23.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -477,8 +530,17 @@
       <c r="J4">
         <v>598.70000000000005</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>2</v>
+      </c>
+      <c r="O4">
+        <v>598.70000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -503,8 +565,17 @@
       <c r="J5">
         <v>17.899999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>3</v>
+      </c>
+      <c r="N5">
+        <v>3</v>
+      </c>
+      <c r="O5">
+        <v>598.70000000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -529,8 +600,18 @@
       <c r="J6">
         <v>254.7</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="M6" s="1"/>
+      <c r="N6">
+        <v>4</v>
+      </c>
+      <c r="O6">
+        <v>23.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -549,8 +630,17 @@
       <c r="G7">
         <v>123.586</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>5</v>
+      </c>
+      <c r="N7">
+        <v>5</v>
+      </c>
+      <c r="O7">
+        <v>17.899999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -569,8 +659,17 @@
       <c r="G8">
         <v>23.88654</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <v>6</v>
+      </c>
+      <c r="N8">
+        <v>6</v>
+      </c>
+      <c r="O8">
+        <v>55.9698899826288</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -589,8 +688,17 @@
       <c r="G9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>7</v>
+      </c>
+      <c r="N9">
+        <v>7</v>
+      </c>
+      <c r="O9">
+        <v>73.869889982628905</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -609,8 +717,17 @@
       <c r="G10">
         <v>2.36029</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <v>8</v>
+      </c>
+      <c r="N10">
+        <v>8</v>
+      </c>
+      <c r="O10">
+        <v>417.86988998262899</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -629,8 +746,17 @@
       <c r="G11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <v>9</v>
+      </c>
+      <c r="N11">
+        <v>9</v>
+      </c>
+      <c r="O11">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -649,8 +775,17 @@
       <c r="G12">
         <v>1.0129999999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <v>10</v>
+      </c>
+      <c r="N12">
+        <v>10</v>
+      </c>
+      <c r="O12">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -669,8 +804,17 @@
       <c r="G13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <v>11</v>
+      </c>
+      <c r="N13">
+        <v>11</v>
+      </c>
+      <c r="O13">
+        <v>417.86988998262899</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -680,8 +824,17 @@
       <c r="C14">
         <v>23.298999999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <v>12</v>
+      </c>
+      <c r="N14">
+        <v>12</v>
+      </c>
+      <c r="O14">
+        <v>417.86988998262899</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -691,8 +844,17 @@
       <c r="C15">
         <v>23.298999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <v>13</v>
+      </c>
+      <c r="N15">
+        <v>13</v>
+      </c>
+      <c r="O15">
+        <v>254.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -702,8 +864,17 @@
       <c r="C16">
         <v>21.435079999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <v>14</v>
+      </c>
+      <c r="N16">
+        <v>14</v>
+      </c>
+      <c r="O16">
+        <v>678.56988998262898</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -713,8 +884,17 @@
       <c r="C17">
         <v>1.0393380000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <v>15</v>
+      </c>
+      <c r="N17">
+        <v>15</v>
+      </c>
+      <c r="O17">
+        <v>678.56988998262898</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -724,8 +904,17 @@
       <c r="C18">
         <v>1.0231300000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <v>16</v>
+      </c>
+      <c r="N18">
+        <v>16</v>
+      </c>
+      <c r="O18">
+        <v>678.56988998262898</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -735,8 +924,17 @@
       <c r="C19">
         <v>123.586</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L19">
+        <v>17</v>
+      </c>
+      <c r="N19">
+        <v>17</v>
+      </c>
+      <c r="O19">
+        <v>132.44026156809699</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -746,8 +944,17 @@
       <c r="C20">
         <v>23.88654</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L20">
+        <v>18</v>
+      </c>
+      <c r="N20">
+        <v>18</v>
+      </c>
+      <c r="O20">
+        <v>132.44026156809699</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -757,8 +964,17 @@
       <c r="C21">
         <v>23.88654</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L21">
+        <v>19</v>
+      </c>
+      <c r="N21">
+        <v>19</v>
+      </c>
+      <c r="O21">
+        <v>132.44026156809699</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -768,8 +984,17 @@
       <c r="C22">
         <v>23.88654</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <v>20</v>
+      </c>
+      <c r="N22">
+        <v>20</v>
+      </c>
+      <c r="O22">
+        <v>76.470371585467902</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -779,8 +1004,17 @@
       <c r="C23">
         <v>2.36029</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L23">
+        <v>21</v>
+      </c>
+      <c r="N23">
+        <v>21</v>
+      </c>
+      <c r="O23">
+        <v>76.470371585467902</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -790,8 +1024,17 @@
       <c r="C24">
         <v>2.0062465</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L24">
+        <v>22</v>
+      </c>
+      <c r="N24">
+        <v>22</v>
+      </c>
+      <c r="O24">
+        <v>76.470371585467902</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -801,8 +1044,17 @@
       <c r="C25">
         <v>1.0129999999999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L25">
+        <v>23</v>
+      </c>
+      <c r="N25">
+        <v>23</v>
+      </c>
+      <c r="O25">
+        <v>55.9698899826288</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -812,8 +1064,17 @@
       <c r="C26">
         <v>130.09052631578899</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L26">
+        <v>24</v>
+      </c>
+      <c r="N26">
+        <v>24</v>
+      </c>
+      <c r="O26">
+        <v>132.44026156809699</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -822,6 +1083,401 @@
       </c>
       <c r="C27">
         <v>23.298999999999999</v>
+      </c>
+      <c r="L27">
+        <v>25</v>
+      </c>
+      <c r="N27">
+        <v>25</v>
+      </c>
+      <c r="O27">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F30E7D00-7974-4310-AD44-1EF16B4174DC}">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection sqref="A1:D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>288.14999999999998</v>
+      </c>
+      <c r="C2">
+        <v>1.0129999999999999</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>288.14999999999998</v>
+      </c>
+      <c r="C3">
+        <v>1.0129999999999999</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>692</v>
+      </c>
+      <c r="C4">
+        <v>23.298999999999999</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>536</v>
+      </c>
+      <c r="C5">
+        <v>23.298999999999999</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>536</v>
+      </c>
+      <c r="C6">
+        <v>23.298999999999999</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>838.65</v>
+      </c>
+      <c r="C7">
+        <v>23.88654</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1073.0999999999999</v>
+      </c>
+      <c r="C8">
+        <v>23.298999999999999</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1173.0999999999999</v>
+      </c>
+      <c r="C9">
+        <v>23.298999999999999</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>692</v>
+      </c>
+      <c r="C10">
+        <v>23.298999999999999</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1073.1500000000001</v>
+      </c>
+      <c r="C11">
+        <v>23.298999999999999</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1940.9</v>
+      </c>
+      <c r="C12">
+        <v>23.298999999999999</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>1737</v>
+      </c>
+      <c r="C13">
+        <v>23.298999999999999</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>692</v>
+      </c>
+      <c r="C14">
+        <v>23.298999999999999</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>1852.9</v>
+      </c>
+      <c r="C15">
+        <v>21.435079999999999</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>1011.5289592875801</v>
+      </c>
+      <c r="C16">
+        <v>1.0393380000000001</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>428.15</v>
+      </c>
+      <c r="C17">
+        <v>1.0231300000000001</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>838.65</v>
+      </c>
+      <c r="C18">
+        <v>123.586</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>586.73382693576605</v>
+      </c>
+      <c r="C19">
+        <v>23.88654</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>838.65</v>
+      </c>
+      <c r="C20">
+        <v>23.88654</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>838.65</v>
+      </c>
+      <c r="C21">
+        <v>23.88654</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>513.46863761679003</v>
+      </c>
+      <c r="C22">
+        <v>2.36029</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>292.14999999999998</v>
+      </c>
+      <c r="C23">
+        <v>2.0062465</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>283.14999999999998</v>
+      </c>
+      <c r="C24">
+        <v>1.0129999999999999</v>
+      </c>
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>321.14999999999998</v>
+      </c>
+      <c r="C25">
+        <v>130.09052631578899</v>
+      </c>
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>536</v>
+      </c>
+      <c r="C26">
+        <v>23.298999999999999</v>
+      </c>
+      <c r="D26" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>